<commit_message>
new test cases for 'create accont functionality'
</commit_message>
<xml_diff>
--- a/docs/test-scenarios-cases.xlsx
+++ b/docs/test-scenarios-cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\amazon-testing-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\amazon-automation-testing\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4235DD8C-2FFB-4076-85B5-0F2FB2C4E38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C84F2F2-1595-4AF3-8508-25371E805A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1110" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="110">
   <si>
     <t>Scenarios</t>
   </si>
@@ -223,8 +223,122 @@
     <t>all fields shall clear</t>
   </si>
   <si>
+    <t>Enter your e-mail meassage shall appear</t>
+  </si>
+  <si>
+    <t>Ensure 'Business Account PAge' page can be accessed from Create Account page</t>
+  </si>
+  <si>
+    <t>Vality the working of Create Account Functionality</t>
+  </si>
+  <si>
+    <t>click 'Help' and make sure help page opens</t>
+  </si>
+  <si>
+    <t>TC_CAF_002</t>
+  </si>
+  <si>
+    <t>TC_CAF_003</t>
+  </si>
+  <si>
+    <t>TC_CAF_004</t>
+  </si>
+  <si>
+    <t>TC_CAF_005</t>
+  </si>
+  <si>
+    <t>TC_CAF_006</t>
+  </si>
+  <si>
+    <t>TC_CAF_007</t>
+  </si>
+  <si>
+    <t>TC_CAF_008</t>
+  </si>
+  <si>
+    <t>TC_CAF_009</t>
+  </si>
+  <si>
+    <t>TC_CAF_010</t>
+  </si>
+  <si>
+    <t>TC_CAF_011</t>
+  </si>
+  <si>
+    <t>TC_CAF_012</t>
+  </si>
+  <si>
+    <t>TC_CAF_013</t>
+  </si>
+  <si>
+    <t>TC_CAF_014</t>
+  </si>
+  <si>
+    <t>TC_CAF_015</t>
+  </si>
+  <si>
+    <t>TC_CAF_016</t>
+  </si>
+  <si>
+    <t>TC_CAF_017</t>
+  </si>
+  <si>
+    <t>TC_CAF_018</t>
+  </si>
+  <si>
+    <t>TC_CAF_019</t>
+  </si>
+  <si>
+    <t>TC_CAF_020</t>
+  </si>
+  <si>
+    <t>TC_CAF_021</t>
+  </si>
+  <si>
+    <t>TC_CAF_022</t>
+  </si>
+  <si>
+    <t>TC_CAF_023</t>
+  </si>
+  <si>
+    <t>TC_CAF_024</t>
+  </si>
+  <si>
+    <t>TC_CAF_025</t>
+  </si>
+  <si>
+    <t>TC_CAF_026</t>
+  </si>
+  <si>
+    <t>TC_CAF_027</t>
+  </si>
+  <si>
+    <t>TC_CAF_028</t>
+  </si>
+  <si>
+    <t>TC_CAF_029</t>
+  </si>
+  <si>
+    <t>TC_CAF_030</t>
+  </si>
+  <si>
+    <t>TC_CAF_031</t>
+  </si>
+  <si>
+    <t>copy password and paste in password again field</t>
+  </si>
+  <si>
+    <t>password do not match' message</t>
+  </si>
+  <si>
+    <t>E-mail address already in use' message</t>
+  </si>
+  <si>
+    <t>"Passwords must consist of at least 6 characters." message</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Enter your name </t>
+      <t xml:space="preserve">Enter your name, Enter your e-mail, Enter your password </t>
     </r>
     <r>
       <rPr>
@@ -236,29 +350,32 @@
     </r>
   </si>
   <si>
-    <t>Enter your e-mail meassage shall appear</t>
-  </si>
-  <si>
-    <t>Enter your password meassage shall appear</t>
-  </si>
-  <si>
-    <t>Type your password again meassage shall appear</t>
-  </si>
-  <si>
-    <t>Ensure 'Business Account PAge' page can be accessed from Create Account page</t>
-  </si>
-  <si>
-    <t>Vality the working of Create Account Functionality</t>
-  </si>
-  <si>
-    <t>click 'Help' and make sure help page opens</t>
+    <t>empty password and password again</t>
+  </si>
+  <si>
+    <t>"Passwords don't match" message</t>
+  </si>
+  <si>
+    <t>"Enter youtr name" meassage</t>
+  </si>
+  <si>
+    <t>"Type your password again" meassage shall appear</t>
+  </si>
+  <si>
+    <t>"Enter your password" meassage shall appear</t>
+  </si>
+  <si>
+    <t>validate account success page opens after creating account</t>
+  </si>
+  <si>
+    <t>validate email is sent after creating account</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,6 +408,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -312,13 +436,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,7 +758,7 @@
         <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -643,10 +769,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D541B4-1FC8-4616-AC31-B1366DD61DCA}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,13 +834,10 @@
       <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -723,12 +846,12 @@
         <v>14</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>65</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
@@ -736,13 +859,13 @@
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>66</v>
+      <c r="G4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
@@ -751,12 +874,12 @@
         <v>17</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
         <v>33</v>
@@ -764,10 +887,13 @@
       <c r="C6" t="s">
         <v>18</v>
       </c>
+      <c r="G6" s="3" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
         <v>34</v>
@@ -775,10 +901,13 @@
       <c r="C7" t="s">
         <v>56</v>
       </c>
+      <c r="G7" s="3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
         <v>35</v>
@@ -786,10 +915,13 @@
       <c r="C8" t="s">
         <v>19</v>
       </c>
+      <c r="G8" s="3" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
         <v>36</v>
@@ -800,7 +932,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
         <v>37</v>
@@ -808,8 +940,14 @@
       <c r="C10" t="s">
         <v>21</v>
       </c>
+      <c r="G10" s="4" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
       <c r="C11" t="s">
         <v>57</v>
       </c>
@@ -819,7 +957,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
         <v>38</v>
@@ -827,8 +965,14 @@
       <c r="C12" t="s">
         <v>22</v>
       </c>
+      <c r="G12" s="3" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>78</v>
+      </c>
       <c r="C13" t="s">
         <v>60</v>
       </c>
@@ -836,152 +980,200 @@
         <v>63</v>
       </c>
     </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C17" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
         <v>39</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C21" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" t="s">
-        <v>46</v>
+        <v>86</v>
+      </c>
+      <c r="C25" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>43</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="B32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
         <v>53</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1036,7 +1228,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>